<commit_message>
Fixed a few bugs on the airport types
</commit_message>
<xml_diff>
--- a/Supporting Documents/Feature Engineering-step3_1.xlsx
+++ b/Supporting Documents/Feature Engineering-step3_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\987\GIT_LHL\DataScienceBootcamp\Projects\LHL_MidTermProject\Supporting Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF1DC447-4281-479B-8C00-4C74A8829D04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D7BE6E-215B-4B31-83E2-237E20374027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="360" windowWidth="19032" windowHeight="16464" xr2:uid="{8BBF7224-E169-4680-9C98-7D67102F622B}"/>
   </bookViews>
@@ -1071,10 +1071,10 @@
   <dimension ref="A1:X89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D9" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L28" sqref="L28"/>
+      <selection pane="bottomRight" activeCell="Q47" sqref="Q47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3729,14 +3729,13 @@
 flights_sample['type_dep'] = scaler.transform(flights_sample[['type_dep']])
 </v>
       </c>
-      <c r="N47" s="18" t="s">
+      <c r="O47" s="13" t="str">
+        <f t="shared" si="5"/>
+        <v>flights_sample = pd.get_dummies(flights_sample, columns=['type_dep'], drop_first=True)</v>
+      </c>
+      <c r="P47" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="O47" s="13" t="str">
-        <f t="shared" si="5"/>
-        <v>flights_sample = pd.get_dummies(flights_sample, columns=['type_dep'], drop_first=True)</v>
-      </c>
-      <c r="P47" s="18"/>
       <c r="Q47" s="13" t="str">
         <f t="shared" si="6"/>
         <v>flights_sample = pd.get_dummies(flights_sample, columns=['type_dep'], drop_first=False)</v>

</xml_diff>

<commit_message>
Nov 30 Melissa edits
</commit_message>
<xml_diff>
--- a/Supporting Documents/Feature Engineering-step3_1.xlsx
+++ b/Supporting Documents/Feature Engineering-step3_1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\987\GIT_LHL\DataScienceBootcamp\Projects\LHL_MidTermProject\Supporting Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mnicn\local_documents\lighthouse-data-notes\Midterm Project\LHL_MidTermProject\Supporting Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D7BE6E-215B-4B31-83E2-237E20374027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C6F201-1B23-46B2-BF5C-7FBA9D852354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="19032" windowHeight="16464" xr2:uid="{8BBF7224-E169-4680-9C98-7D67102F622B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{8BBF7224-E169-4680-9C98-7D67102F622B}"/>
   </bookViews>
   <sheets>
     <sheet name="Take 2" sheetId="2" r:id="rId1"/>
@@ -1071,10 +1071,10 @@
   <dimension ref="A1:X89"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="E21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q47" sqref="Q47"/>
+      <selection pane="bottomRight" activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1083,17 +1083,17 @@
     <col min="3" max="3" width="28.5546875" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.33203125" style="17" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="19" customWidth="1"/>
     <col min="7" max="7" width="4.6640625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="8.77734375" style="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" style="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="4.6640625" style="30" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="4.6640625" style="33" customWidth="1"/>
-    <col min="12" max="12" width="16" style="19" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.88671875" style="19" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="4.6640625" style="14" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" style="19" customWidth="1"/>
+    <col min="14" max="14" width="26.109375" style="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="4.6640625" style="14" customWidth="1"/>
-    <col min="16" max="16" width="17.88671875" style="19" customWidth="1"/>
+    <col min="16" max="16" width="26.44140625" style="19" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="4.6640625" style="14" customWidth="1"/>
     <col min="18" max="18" width="16.88671875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="13.77734375" bestFit="1" customWidth="1"/>

</xml_diff>